<commit_message>
modified the business payment
</commit_message>
<xml_diff>
--- a/VINAYTECH_BUSINESS_PAYMENT_DETAILS_DATAMODEL_DATASET.xlsx
+++ b/VINAYTECH_BUSINESS_PAYMENT_DETAILS_DATAMODEL_DATASET.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mahesh\mahesh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\mahesh_training_data-test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729E881C-B82F-4F79-A66F-4AD7279D4677}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28306C45-8F12-4E7D-82AB-1F9986ED79EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4919" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4920" uniqueCount="674">
   <si>
     <t>30.04.2007 16:53:36</t>
   </si>
@@ -2064,6 +2064,9 @@
   </si>
   <si>
     <t>vijaya mahesh training institute</t>
+  </si>
+  <si>
+    <t>Today class is pending</t>
   </si>
 </sst>
 </file>
@@ -8434,10 +8437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8499,6 +8502,11 @@
         <v>672</v>
       </c>
       <c r="C5" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>673</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
seond time modified business data
</commit_message>
<xml_diff>
--- a/VINAYTECH_BUSINESS_PAYMENT_DETAILS_DATAMODEL_DATASET.xlsx
+++ b/VINAYTECH_BUSINESS_PAYMENT_DETAILS_DATAMODEL_DATASET.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\mahesh_training_data-test1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\mahesh_training_data-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28306C45-8F12-4E7D-82AB-1F9986ED79EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9266739-E890-4D4A-98AD-4D141FF1768F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4920" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4923" uniqueCount="677">
   <si>
     <t>30.04.2007 16:53:36</t>
   </si>
@@ -2067,6 +2067,15 @@
   </si>
   <si>
     <t>Today class is pending</t>
+  </si>
+  <si>
+    <t>vijaya</t>
+  </si>
+  <si>
+    <t>mahesh</t>
+  </si>
+  <si>
+    <t>supriya</t>
   </si>
 </sst>
 </file>
@@ -8437,10 +8446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8506,6 +8515,21 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>